<commit_message>
add roles & ver4
</commit_message>
<xml_diff>
--- a/reports - 複製.xlsx
+++ b/reports - 複製.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/202a4d3f52753dd9/Desktop/CUHK/Applied Deep Learning/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="11_6516D9635E53C5551074CBD6A40F17EACCE3ADEE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{462E2386-3E18-49AA-A71F-9D609918A97C}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_34FCE11E4DA35EC193CC7A0D7AC9251CE07AE52D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE2E7D02-DAAB-4E04-B296-ED7116311BC4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2964" yWindow="2964" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -24,83 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+  <si>
+    <t>ver1</t>
+  </si>
   <si>
     <t>ver2</t>
   </si>
   <si>
-    <t># Financial Analysis Report
-## Company Overview
-China Longyuan Power Group Corporation Limited is a leading player in the renewable energy sector, especially focusing on wind and photovoltaic power. The company is strategically positioned to leverage China's transition towards sustainable energy sources. In the first half of 2024, China’s economy experienced a stable growth trajectory, with GDP increasing by 5.0% year-on-year. This economic backdrop supports the company's initiatives, primarily aimed at expanding renewable energy capacity and enhancing operational efficiencies. The company’s strategic emphasis on innovation, talent development, and environmental sustainability aligns with global trends towards green energy adoption.
-## Revenue Structure
-The revenue structure of China Longyuan Power for the first half of 2024 included various segments, such as energy storage equipment rental, repair services, sales of commodity materials, and miscellaneous income. While specific revenue figures were not disclosed for each component, the overall operating profit from these activities reached RMB 101 million—a notable increase of RMB 93 million compared to the same period in 2023. This growth was primarily driven by the company's diversified revenue streams, underlining its commitment to optimizing its financing structure to support revenue-generating activities. However, the report also highlighted challenges in domestic demand that could potentially stifle future revenue growth.
-## Profit
-The company’s net profit performance can be assessed against the backdrop of China's stable economic growth. Despite the favorable conditions, the company faces challenges stemming from insufficient domestic demand and the need for a consolidated economic recovery. These factors could impact net profit sustainability over time. The strategic focus on building a world-class new energy asset management platform aims to capitalize on emerging market opportunities, even as external complexities present potential risks to profitability in the near term.
-## Valuation
-As of June 30, 2024, the company's total liabilities amounted to RMB 80,011 million, with total equity attributable to equity holders at RMB 72,658 million, yielding a debt-to-equity ratio of approximately 1.10. This ratio indicates that the company operates with a relatively leveraged financial position. The valuation metrics suggest that while the company is growing, its reliance on debt financing could pose risks, particularly in a fluctuating economic environment. 
-## Summary
-In summary, China Longyuan Power is navigating a complex economic landscape characterized by growth in renewable energy demand and significant challenges in achieving domestic sales targets. While the revenue structure shows promise through diverse streams, the company's reliance on coal and thermal power raises concerns about sustainability. The focus on enhancing operational efficiency and expanding renewable capacity is crucial for maintaining competitive advantage.
-## Future Outlook
-Looking ahead, China Longyuan Power aims to expand its installed capacity, building on the success of adding 2,286.73 MW across 47 new projects in the first half of 2024. The company’s commitment to optimizing management practices for its existing assets and enhancing its renewable energy portfolio aligns with industry trends towards sustainability. However, it must also navigate external factors such as fluctuating fuel prices, regulatory changes, and market competition which could disrupt growth strategies.
-## Factors Affecting Revenue
-Key factors influencing the company's electricity sales revenue include the introduction of a time-of-use electricity fee policy, which introduces price volatility. The targeted utilization rate for new energy sources aims to remain above 90%, though regional disparities in resource conditions may challenge this goal. Moreover, the pricing mechanisms for ancillary services and fluctuations in coal prices significantly affect electricity sales revenue. 
-## Installed Capacity Trends
-As of June 30, 2024, the company’s consolidated installed capacity reached 37,880.40 MW, reflecting growth attributed to new wind and photovoltaic projects. The expansion in renewable energy infrastructure, particularly photovoltaic technology, is a positive trend for the company, positioning it well for future energy production demands. 
-## Electricity Sales Performance
-In the first half of 2024, total electricity sales declined by 2.39% year-on-year, amounting to 4,907,935 MWh. This decline is attributed to increased competition from new energy capacity in regions like Jiangsu, which has affected coal power generation. The average utilization hours for coal power also fell by 64 hours year-on-year, indicating challenges in maintaining revenue from conventional energy sources.
-## Operational Costs and Profit Margins
-The increase in operational costs, primarily driven by higher personnel expenses and maintenance costs, emphasizes the need for improved efficiency. The operating expenses rose to RMB 2,358 million, reflecting an 8.1% increase compared to the previous year. These pressures on operational costs could negatively impact net profit margins unless effectively managed through strategic cost allocation and operational optimization.
-## Risks and Mitigation Strategies
-The company has identified several operational risks, including weaknesses in grid infrastructure and price volatility from time-of-use electricity fees. To mitigate these risks, the company has implemented robust safety management systems and proactive financial risk assessments, especially concerning foreign exchange and fuel price fluctuations. 
-## Capital Expenditures and Financial Stability
-Increased capital expenditures have implications for financial stability, particularly if funded through debt. The company's approach to capital management, including the integration of newly acquired subsidiaries, further demonstrates a focus on maintaining a steady financial position while pursuing growth opportunities.
-## Regulatory Environment
-The regulatory landscape plays a crucial role in shaping the company’s operations and financial planning. Compliance with accounting standards and adherence to policies regarding renewable energy development are fundamental to the company's strategy and financial reporting processes.
-## Stakeholder Communication
-China Longyuan Power effectively communicates its value proposition to stakeholders by emphasizing its commitment to sustainable growth and innovation. This approach not only strengthens stakeholder relationships but also reinforces the company's market position as a leader in the transition to renewable energy.
-## Conclusion
-In conclusion, China Longyuan Power Group Corporation Limited stands at a pivotal point in its growth trajectory, balancing the opportunities presented by China’s commitment to renewable energy with the challenges of market volatility and operational efficiency. Strategic investments, effective risk management, and a focus on sustainable practices will be essential for the company to navigate the evolving energy landscape and achieve its long-term objectives.</t>
-  </si>
-  <si>
-    <t># JNBY Financial Analysis Report
-## Company Overview
-JNBY, an influential designer fashion house based in China, has been operational for nearly three decades, establishing itself as a prominent player in the contemporary apparel market. The company's diverse brand portfolio includes established names like JNBY, along with younger and emerging brands such as CROQUIS, jnby by JNBY, and POMME DE TERRE. This segmentation allows JNBY to effectively target distinct customer demographics with tailored products, ranging from apparel to footwear and household items. As of June 30, 2024, JNBY has adapted to the evolving landscape of digital consumption and e-commerce, reflecting a commitment to quality and customer experience. This adaptation is critical, given the growing trend of consumers gravitating towards trusted brands that offer personalized experiences.
-## Revenue Structure
-JNBY's revenue structure is significantly influenced by its diversified brand portfolio and sales channels. The company primarily generates revenue from offline retail outlets and online platforms, with Tmall.com being a notable third-party platform for e-commerce. For the fiscal year ending June 30, 2024, JNBY reported total revenue of RMB 5,238,149, marking a 17.3% increase from RMB 4,465,124 in the previous year. This growth can be attributed to both the expansion of standalone retail stores from 1,990 to 2,024 and a notable increase in same-store sales. The integration of a loyalty program has further enhanced revenue generation by encouraging repeat purchases, indicating that JNBY is effectively leveraging both its physical and digital sales channels.
-## Profit
-In terms of profitability, JNBY has demonstrated strong performance metrics. The company's gross profit for the same fiscal year increased to RMB 3,470,485 from RMB 2,916,992, reflecting a growth rate of approximately 19%. This outpaced revenue growth, suggesting improved operational efficiency and effective cost management strategies. Notably, JNBY's operating profit surged to RMB 1,194,266, a remarkable increase of 39.5% from RMB 857,898 in the prior year. This indicates a favorable trend in profitability, as the net profit growth significantly outpaced gross profit growth, showcasing the company's ability to capitalize on increased sales while managing expenses effectively.
-## Valuation
-The valuation of JNBY can be inferred through its financial performance indicators and market positioning. The increasing trend in dividends, with a total payout of HK$1.71 per ordinary share for the 2024 fiscal year, signals confidence in sustained growth and profitability. This includes a final dividend of HK$0.86, an interim dividend of HK$0.46, and a special interim dividend of HK$0.39, representing a clear commitment to returning value to shareholders. The overall increase in dividends compared to the previous fiscal year aligns with JNBY's focus on high-quality development and reflects the company's positive outlook on consumption growth.
-## Summary
-Overall, JNBY's financial performance for the fiscal year ending June 30, 2024, demonstrates resilience and adaptability in a competitive market. The company's revenue growth, coupled with substantial increases in both gross and operating profits, highlights effective management strategies and a commitment to operational excellence. JNBY's diversified brand portfolio and multi-channel sales approach position it favorably in the evolving fashion landscape, where consumer preferences are shifting towards sustainability and personalized experiences. 
-## Future Outlook
-Looking ahead, JNBY's management anticipates continued revenue growth, driven by the stabilization of China's economy and a renewed focus on expanding domestic demand. Enhanced consumer confidence is expected to bolster sales, particularly as the company adapts to changing consumer behaviors through its "design-driven" approach and multi-brand strategies. Additionally, JNBY's emphasis on sustainability and social responsibility is likely to resonate with younger consumers, further enhancing its market position.
-Strategically, JNBY plans to recruit talent with expertise in brand management to support its expansion into new product categories, including children's apparel and household goods. This diversification, alongside their commitment to quality and innovative design, positions JNBY for sustainable growth in the coming years.
-## Other Details
-JNBY's commitment to sustainability is evident through its focus on eco-friendly materials and supplier management practices that prioritize green energy. The company has engaged actively in industry discussions on sustainable development, indicating its alignment with global trends toward responsible consumption. Financially, JNBY's proactive risk management strategies, including its approach to market and operational risks, contribute to its resilience against external shocks.
-In conclusion, JNBY is well-positioned for future growth, supported by a robust financial framework, a commitment to sustainability, and an adaptive approach to market changes. The company's focus on innovation, customer engagement, and operational efficiency will be key to navigating the competitive landscape and achieving long-term success.</t>
-  </si>
-  <si>
-    <t># Financial Analysis Report: China Tobacco International (HK) Company Limited
-## 1. Company Overview
-China Tobacco International (HK) Company Limited (CTIHK) functions as a pivotal subsidiary of the China National Tobacco Corporation (CNTC). It specializes in the import and export of tobacco leaf products, thereby playing a critical role in international trade within the tobacco industry. In 2024, CTIHK engaged in substantial transactions, recording HK$1,461.3 million under its tobacco purchase agreements. This figure highlights the company's robust operational capacity and strategic significance within CNTC's broader framework. The company's ownership structure indicates a significant relationship with its parent entity, China Tobacco International Group (CTIG), which suggests that CTIG likely exerts considerable control over CTIHK's operations.
-## 2. Revenue Structure
-CTIHK’s revenue is primarily derived from its Tobacco Leaf Products Export and Import businesses. In the first half of 2024, the Tobacco Leaf Products Import Business reported total revenue of HK$6,802.2 million, representing the entirety of its revenue stream. This indicates a well-structured business model that focuses on long-term supply agreements with strategic partners such as Alliance One Brazil. The export segment further diversifies revenue, targeting key markets including Southeast Asia, Hong Kong, Macau, Taiwan, and Europe. The sales dynamics demonstrate the company's ability to adapt its offerings to meet market demands effectively.
-## 3. Profit
-The company achieved a remarkable 33% increase in profit for the period, amounting to HK$679,702 million, up from HK$510,540 million in the previous year. Despite this growth in profit, there was a noted decline in gross profit margins due to a shift in product sales towards finished tobacco strips, which, although higher in unit price, offered lower gross margins compared to traditional tobacco leaf by-products. The total sale transactions during the reporting period reached HK$184.0 million, further underscoring CTIHK's operational performance amidst changing market dynamics.
-## 4. Valuation
-While specific valuation metrics for CTIHK relative to industry standards are not detailed within the retrieved context, the company’s profitability, along with its substantial revenue figures, suggests a potentially favorable valuation position. Typically, valuation assessments involve analyzing price-to-earnings (P/E) ratios, price-to-sales (P/S) ratios, and enterprise value-to-EBITDA (EV/EBITDA) ratios. The increase in profit and revenue, coupled with strategic growth plans, positions CTIHK favorably within the market, likely leading to a positive outlook on its valuation in the tobacco sector.
-## 5. Summary
-In summary, CTIHK has positioned itself as a significant player in the international tobacco market through its comprehensive procurement, export, and import operations. The company's financial performance has been robust, highlighted by a notable increase in profit alongside strategic revenue generation from both its export and import businesses. However, challenges remain, particularly concerning gross profit margins, which require close monitoring and strategic adjustments to ensure sustained profitability.
-## 6. Future Outlook
-Looking ahead, CTIHK anticipates continued growth driven by its strategic focus on both organic and inorganic development. The company's commitment to enhancing its market presence through innovative product offerings, particularly in the new tobacco products segment, signals a proactive approach to capturing market share. The increase in revenue from new tobacco products, from HK$33,895,000 in 2023 to HK$43,517,000 in 2024, reflects the company's adaptability to consumer trends. Furthermore, the absence of export tariffs for new tobacco products is expected to bolster competitiveness in international markets.
-## 7. Operational and Strategic Insights
-CTIHK's operational strategy is underpinned by a diversified supply chain management approach, allowing for effective resource allocation across its various business segments. The company engages in rigorous market analysis to adapt its pricing strategies based on supply chain dynamics, customer demand, and market conditions. This flexible approach is critical in managing fluctuations in procurement costs and maintaining profitability.
-Moreover, CTIHK's emphasis on corporate governance enhances its operational transparency and compliance with regulatory standards. The company’s adherence to the Hong Kong Financial Reporting Standards (HKFRS) and the Companies Ordinance demonstrates a commitment to maintaining high standards of corporate governance, which is vital for fostering stakeholder trust.
-## 8. Performance Monitoring and Risk Management
-CTIHK employs a structured performance monitoring system through segment reporting that evaluates the revenue from different product lines and geographical regions. This allows for a granular assessment of profitability and operational efficiency. The company is also aware of potential risks, including fluctuations in global tobacco supply, regulatory changes, and shifting consumer preferences towards alternative products. To mitigate these risks, CTIHK engages in long-term partnerships with approved suppliers, ensuring a stable supply chain and consistent product quality.
-## 9. Conclusion
-In conclusion, China Tobacco International (HK) Company Limited is strategically positioned within the global tobacco industry, demonstrating robust financial performance amid evolving market conditions. The company’s focus on sustainable growth through innovative product development and strategic partnerships enables it to navigate challenges while capitalizing on emerging opportunities. As it continues to adapt to changing consumer demands and market dynamics, CTIHK is well-positioned for sustained success in the years to come.</t>
+    <t>ver3</t>
   </si>
   <si>
     <t># Financial Analysis Report: CK Hutchison Holdings Limited
@@ -119,30 +51,40 @@
 ## 7. Additional Insights
 CK Hutchison navigates various external influences that impact its performance, including regulatory changes, competitive dynamics, and economic factors. The company's geographic diversification aids in stabilizing revenue streams across different markets, allowing it to mitigate risks associated with regional downturns. Operational risks, particularly in the telecommunications sector, require ongoing attention to regulatory compliance and market adaptability. Furthermore, geopolitical factors, including trade tensions and currency fluctuations, could affect CK Hutchison's supply chain and financial performance.
 In conclusion, CK Hutchison's commitment to sustainable earnings, strategic diversification, and disciplined financial management positions it well for future growth. As the company continues to adapt to changing market conditions and consumer preferences, its focus on innovation and technology transformation will be critical in maintaining its competitive edge. Stakeholder engagement and corporate governance remain integral to its strategy, ensuring alignment with the interests of investors, customers, and regulatory bodies.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t># Financial Analysis Report of CK Hutchison Holdings Limited
+  </si>
+  <si>
+    <t># CK Hutchison Financial Analysis Report
 ## Company Overview
-CK Hutchison Holdings Limited operates as a diversified multinational conglomerate with a primary business structure organized into four core segments: ports and related services, retail, infrastructure, and telecommunications. This segmentation allows senior executive management to monitor performance and allocate resources effectively, which enhances strategic decision-making within each core area. By leveraging its extensive management experience across sectors and geographies, the company pursues organic growth while actively engaging in merger and acquisition activities to further diversify its operations.
+CK Hutchison Holdings Limited is a diversified multinational conglomerate operating across various sectors, including telecommunications, e-commerce, infrastructure, and healthcare. The company consolidates its telecommunications operations under CK Hutchison Group Telecom, which has a significant footprint in Europe and holds a substantial stake in Hutchison Telecommunications Hong Kong Holdings. In addition to telecommunications, CK Hutchison is heavily involved in e-commerce through Hutchison E-Commerce and retail through the Marionnaud brand. The group's investments extend into infrastructure assets, including Northumbrian Water and Australian Gas Networks, while its healthcare interests are represented by Hutchison China MediTech and various liquid asset investments.
 ## Revenue Structure
-The company’s revenue structure is categorized into traditional service offerings while also expanding into new revenue streams. The telecommunications segment, for instance, has seen growth through active customer base expansion and new offerings, including cybersecurity and insurance products. In contrast, its retail segment faces challenges due to a mix of low-margin Internet of Things (IoT) customers and inflation-linked customer contract adjustments. Revenue performance varies significantly across geographical regions, with Sweden experiencing a 6% increase in total margin driven by customer growth, while Hutchison Telecommunications Hong Kong encountered a 12% decline in total revenue due to shifting consumer spending patterns.
+CK Hutchison categorizes its revenue-generating segments into telecommunications, e-commerce, retail, and investments in listed companies. The key segments include Hutchison Whampoa (China), Hutchison E-Commerce, and associated entities such as Hutchison China MediTech and Cenovus Energy. In the first half of 2024, the company reported a total revenue of HK$91,469 million, marking a 3% increase in reported currency and a 5% increase in local currencies. The finance and investments segment has emerged as a significant contributor to revenue, particularly propelled by the performance of Cenovus Energy and Indosat Ooredoo Hutchison.
 ## Profit
-Profitability across CK Hutchison's segments has shown mixed results. The company reported a 5% increase in EBITDA, reflecting operational improvements in its Ports and telecommunications divisions. However, the infrastructure segment has faced challenges, notably due to a tariff reset and rising energy costs in the UK and Europe, which have negatively impacted revenue and profit margins. The retail segment's performance is also under scrutiny, particularly in Health and Beauty China, where comparable store sales declined by 19%. Overall, while some segments thrive, others struggle, highlighting the necessity for disciplined management of costs and margins to enhance long-term returns for stakeholders.
+CK Hutchison's profit metrics indicate a stable financial performance, with EBITDA remaining flat at HK$7,089 million and EBIT at HK$5,433 million in reported currency. Despite the challenges faced in various segments, the retail division reported a remarkable 22% revenue growth in the first half of 2024, showcasing effective cost controls amidst rising energy costs and soft consumer demand. The overall profit growth reflects the company's ability to offset underperformance in other areas, such as container shipping.
 ## Valuation
-Valuation metrics indicate that CK Hutchison Holdings Limited maintains a solid financial profile, with a total capital ratio improving to 17.1% from 16.2%. This improvement suggests stronger financial health and stability. The company's focus on achieving recurring and sustainable earnings supports its valuation, alongside its commitment to maintaining long-term investment-grade ratings. However, challenges remain in certain segments, which could influence market perceptions and future valuations. The group’s strategic investments in technology and infrastructure aim to bolster its overall market position, ensuring that valuation remains aligned with long-term growth prospects.
+The valuation of CK Hutchison is influenced by its diversified portfolio and strategic interests. The debt-to-capital ratio as of June 30, 2024, stands at 9.8%, indicating a conservative leverage position that enhances the company's creditworthiness. With a look-through net debt to net total capital ratio of 47.8%, CK Hutchison demonstrates effective management of its infrastructure investments. While specific price-to-earnings and price-to-book ratios are not disclosed, the company's commitment to maintaining strong financial health and shareholder returns suggests a valuation approach that balances risk and growth potential.
 ## Summary
-In summary, CK Hutchison Holdings Limited exhibits a diverse business model with segmented operations that allow for targeted management and strategic growth. While the company has achieved substantial growth in certain areas, it faces challenges in others, particularly in its retail and infrastructure segments. The mixed performance underscores the necessity for ongoing evaluation of market conditions and operational efficiencies, alongside proactive measures to enhance profitability across divisions.
+CK Hutchison's financial performance in the first half of 2024 reflects a combination of revenue growth and disciplined cost management. The retail segment's robust growth is crucial for sustaining the company's profitability, especially amid challenges in other sectors. The telecommunications segment remains a vital part of the overall revenue structure, although it faces competitive pressures. The company's diversified operations across various geographical regions help mitigate risks and contribute to its financial stability.
 ## Future Outlook
-Looking ahead, CK Hutchison Holdings Limited is poised to navigate a complex market landscape characterized by economic uncertainties and competitive pressures. The demand outlook remains positive for the third quarter, although a gradual slowdown is anticipated due to frontloaded cargo orders for the holiday season. The company plans to leverage its strengths in technology transformation and operational enhancements to capture new revenue opportunities, particularly in sectors where it has established management expertise and resources. Additionally, the emphasis on sustainability through initiatives like decarbonization and the "Equipment Electrification Directive" reflects the company’s commitment to align its operations with evolving market demands.
-## Other Details
-Key performance indicators are essential for CK Hutchison's ongoing evaluation of its business segments, with a focus on recurring earnings, cash flow, and dividend growth. Management’s disciplined approach to revenue growth, margin management, and cost control will be pivotal in addressing ongoing market challenges. Furthermore, the company's proactive stance on regulatory compliance and risk management enhances its resilience and adaptability in an ever-evolving global marketplace.
-In conclusion, CK Hutchison Holdings Limited's strategic priorities for growth, combined with its commitment to operational efficiency and sustainability, position the company favorably for future success. As it continues to adapt to changing market dynamics, the company must remain vigilant in managing its weaknesses, particularly in the infrastructure and retail segments, to ensure sustained profitability and shareholder value.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ver1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+Looking ahead, CK Hutchison anticipates moderate volume growth, particularly in the telecommunications segment within Asia, Europe, and Latin America. The management's focus on enhancing margins and reducing costs aims to bolster profitability despite ongoing market challenges. Management is optimistic about the retail segment's performance, driven by increased consumer demand and new revenue streams. However, the company remains cautious about potential slowdowns, particularly in the fourth quarter.
+## Geographic Diversification and Its Impact
+CK Hutchison's extensive geographic diversification plays a vital role in stabilizing its overall performance. The company's operations across approximately 50 countries allow it to leverage local expertise and adapt to specific market conditions. This diversification strategy is essential for generating sustainable earnings and mitigating risks associated with economic downturns in individual regions. The anticipated moderate growth in 2024 highlights the importance of regional economic recovery in shaping CK Hutchison's financial outlook.
+## Challenges in the Chinese Market
+The company faces significant challenges in the Chinese market, particularly with a 19% decline in comparable store sales in the Health and Beauty sector. Factors such as soft consumer demand, increased competition, and broader economic pressures contribute to this downturn. To improve performance in China, CK Hutchison must navigate these challenges while leveraging its diverse business model to enhance resilience.
+## Trends in the Retail Segment
+The retail segment illustrates a positive trend, with revenue growth driven by new streams such as cybersecurity, energy, and insurance products. The segment's EBITDA has increased by 11% in local currency, showcasing improved operational efficiency. However, a decrease in EBIT by 8% due to higher depreciation and amortization highlights the need for continued focus on managing costs while capitalizing on demand.
+## Impact of Currency Fluctuations
+Currency fluctuations pose a significant risk to CK Hutchison's financial performance. As the company operates in various international markets, changes in exchange rates can affect the value of revenues and costs. The Group's treasury function is crucial in managing foreign exchange risks to mitigate potential losses from adverse currency movements, ensuring stable financial outcomes.
+## Operational Risks
+CK Hutchison faces several operational risks, particularly fluctuations in consumer demand and changes in regulatory environments. The 19% decline in sales in China emphasizes the need for agile responses to market dynamics. Additionally, supply chain disruptions could affect inventory levels and service delivery, posing challenges in maintaining consistent performance across sectors.
+## Competitive Landscape
+Competition influences CK Hutchison's strategy by necessitating diversification and adaptation in its various sectors. The company's ownership of multiple businesses enables it to leverage synergies and compete effectively. The leadership structure promotes flexibility and responsiveness to market dynamics, ensuring that CK Hutchison remains proactive in navigating competitive pressures.
+## Corporate Governance and Stakeholder Engagement
+CK Hutchison emphasizes a robust corporate governance framework to enhance shareholder value. Effective stakeholder engagement fosters alignment with financial and operational goals, contributing to the company's reputation and long-term sustainability. Transparency and accountability remain central to CK Hutchison's approach, ensuring that stakeholders are informed and engaged in the company's strategic direction.
+## Sustainability Initiatives
+While specific sustainability initiatives are not detailed in the provided context, CK Hutchison's commitment to sustainability is evident through its focus on environmental, social, and governance (ESG) efforts. The introduction of the Equipment Electrification Directive reflects a significant move towards decarbonization, indicating a forward-thinking approach to sustainability in its operations.
+## Conclusion
+CK Hutchison's financial analysis reveals a company navigating a complex landscape of opportunities and challenges. The diversified portfolio, strong revenue growth in key segments, and prudent financial management position the company favorably for future growth. However, ongoing challenges in specific markets, particularly China, necessitate careful strategic planning and execution. The company's commitment to sustainability, corporate governance, and stakeholder engagement further enhances its potential for long-term success.
+In summary, CK Hutchison's overall sentiment regarding future business prospects remains cautiously optimistic, with an emphasis on disciplined cost management and revenue generation strategies. As the company continues to adapt to changing market conditions, its resilience and strategic positioning will be vital in achieving sustained financial performance and shareholder returns.</t>
   </si>
   <si>
     <t># Financial Analysis Report: Fortune REIT
@@ -172,7 +114,49 @@
 Moving forward, it is recommended that Fortune REIT further strengthen its asset enhancement initiatives, enhance digital marketing strategies to attract tenants, and continue monitoring market trends to identify growth opportunities. Additionally, ongoing engagement with community stakeholders will be crucial in adapting to evolving consumer preferences and ensuring the trust remains a competitive player in the retail sector.
 ## Final Thoughts
 The analysis of Fortune REIT underscores the significance of strategic planning and effective management in navigating the challenges of the retail real estate landscape. As the company prepares for its next reporting period, the focus on transparency, governance, and operational efficiency will be essential in delivering sustained returns for unitholders and enhancing the trust's overall market position.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>### Financial Analysis Report: Fortune REIT
+#### 1. Company Overview
+Fortune REIT is a prominent real estate investment trust (REIT) primarily focused on the management and operation of retail properties. It operates under a structured governance framework designed to ensure accountability, transparency, and effective risk management. Managed by ESR Asset Management (Fortune) Limited, part of the ESR Group, Fortune REIT aligns its strategies with the interests of its investors, notably Cheung Kong Holdings, which holds a significant 33.34% stake in the REIT. The organization emphasizes compliance with the REIT Code, the Securities and Futures Ordinance (SFO), and the Listing Rules, ensuring that mandatory disclosure obligations are met and that shareholder value is maximized within a regulated environment.
+#### 2. Revenue Structure
+In the first half of 2024, Fortune REIT reported a gross revenue of HK$871.8 million, reflecting a 4.1% decrease from HK$908.7 million in the same period in 2023. This decline was primarily driven by negative rental reversions in specific sectors, particularly real estate agencies and supermarkets. The net property income also fell by 5.8% year-on-year to HK$633.1 million from HK$671.9 million. The overall cost-to-revenue ratio increased to 25.1% from 23.8%, indicating rising operational costs amidst declining revenues. Such trends underscore the challenges faced in the retail market, which is still recovering from the impacts of economic fluctuations and changing consumer preferences.
+#### 3. Profit
+Fortune REIT's profit metrics reveal a concerning trend as the net property income, defined as the income generated from retail properties after deducting property-related expenses, declined to HK$633.1 million. The property operating expenses increased by 1.4% to HK$219.1 million, further straining profitability. The overall retail sales value decreased by 6.6%, exacerbating the impact on rental income and contributing to the increased cost-to-income ratio. These financial indicators reflect the challenges faced by the REIT in maintaining profitability amidst a competitive and evolving retail landscape.
+#### 4. Valuation
+The current valuation of Fortune REIT’s properties remains stable, with capitalization rates holding steady at 4.3%. However, the total investment property value slightly decreased from HK$38.439 billion to HK$38.167 billion. This marginal decline indicates potential vulnerabilities in the property valuation due to market dynamics. The management’s proactive strategies to enhance property values, such as the HK$300 million investment in +WOO Phase 2, aim to rejuvenate the asset portfolio and potentially drive future appreciation. Nevertheless, external factors like interest rate changes could significantly impact financing costs and overall property valuations.
+#### 5. Summary
+The financial performance of Fortune REIT in the first half of 2024 illustrates a decline in both revenue and net property income, driven by various market challenges. The necessary emphasis on effective governance, adherence to regulatory frameworks, and strategic asset management remains vital in navigating these circumstances. With a focus on enhancing tenant mix and occupancy rates, the REIT is working to stabilize its financial health despite the observed downturn in profitability.
+#### 6. Future Outlook
+Looking ahead, Fortune REIT faces a mixed outlook. While the occupancy rate has shown slight improvement to 94.8%, the retail sector in Hong Kong remains under pressure from economic fluctuations and changing consumer behaviors. The REIT's long-term strategy includes diversifying its tenant mix to include more lifestyle and entertainment offerings, which aligns with evolving community needs. Additionally, government initiatives aimed at boosting retail demand may provide further support. However, challenges such as negative rental reversions in certain sectors could continue to influence rental income stability.
+#### 7. Additional Details
+Fortune REIT's approach towards maintaining high property standards involves engaging independent external valuers for regular assessments, ensuring transparency and accuracy in property valuations. The focus on community-related tenants has enhanced the shopping experience and attracted diverse demographics, contributing to an increased occupancy rate. Furthermore, effective management of operational costs, alongside strategic leasing agreements, is crucial for sustaining profitability. Investor relations are strengthened through transparency in financial reporting and regular updates on corporate governance practices, fostering trust and confidence among stakeholders.
+In conclusion, while Fortune REIT is navigating a challenging environment marked by fluctuating revenues and competitive pressures, its proactive governance and strategic initiatives position it for resilience and potential growth in the evolving retail landscape.</t>
+  </si>
+  <si>
+    <t># Financial Analysis Report for Fortune REIT
+## Company Overview
+Fortune REIT is a real estate investment trust (REIT) focused on delivering regular and stable returns to its unitholders through the proactive management of its portfolio of assets. Established in 2003, the REIT has grown its asset portfolio to HK$38.7 billion, comprising 17 retail properties, including 16 located in Hong Kong and one in Singapore. The company operates under a governance framework that emphasizes accountability and transparency, with a board that convenes quarterly to review financial performance and strategic decisions. Stakeholders can trust that the REIT is compliant with relevant regulations while aiming to maximize value for its investors.
+## Revenue Structure
+In the first half of 2024, Fortune REIT reported a gross revenue of HK$871.8 million, reflecting a decline of 4.1% from HK$908.7 million during the same period in the previous year. This downturn is attributed to negative rental reversions experienced mainly by real estate agencies and supermarkets. The retail environment in Hong Kong has been challenging, with total retail sales value dropping by 6.6% year-on-year, which remains 22.7% lower than pre-2018 levels. Despite a notable increase in tourist arrivals by 64%, consumer spending has been adversely affected by the strong Hong Kong dollar. This mixed landscape emphasizes the difficulties faced by the retail sector.
+## Profit
+Net Property Income (NPI), defined as total rental income minus property-related expenses, serves as a key indicator of profitability for Fortune REIT. In the first half of 2024, NPI fell by 5.8% due to a rise in operational expenses, even as rental income saw a slight increase of 1.4% year-on-year, totaling HK$219.1 million. The cost-to-income ratio in the Hong Kong retail market has been under pressure, driven by declining total retail sales and increased competition. While the occupancy rate has shown an upward trend, rising to 94.8% from 94.4%, the overall rental income stability remains challenged.
+## Valuation
+Fortune REIT's market yield, or capitalization rate, is affected by various factors, including property income fluctuations and market dynamics. The integration of management and governance structures, notably influenced by Cheung Kong Holdings, which holds a 33.3% stake, enables effective decision-making that aligns with long-term strategic goals. The company's valuation reflects its robust portfolio and proactive management, although ongoing challenges in the rental market may necessitate adjustments to property valuations.
+## Summary
+The financial performance of Fortune REIT in the first half of 2024 highlights the challenges within the Hong Kong retail sector, characterized by declining revenues and shifts in consumer behavior. The REIT's proactive management strategies, however, have maintained relatively stable occupancy rates and tenant retention at 83%. The emphasis on asset enhancement initiatives and community-oriented tenant structures aims to bolster resilience and vibrancy within its retail spaces.
+## Future Outlook
+Looking ahead, Fortune REIT intends to adapt to changing market conditions by focusing on strategic acquisitions and enhancing the tenant mix within its portfolio. The company is well-positioned to leverage its strong balance sheet, which enables it to withstand market fluctuations and capitalize on growth opportunities. The anticipated increase in occupancy rates, particularly in renovated spaces, coupled with ongoing asset enhancement initiatives, is expected to drive revenue recovery in the latter half of 2024.
+## Additional Analysis
+Considering the implications of interest rate fluctuations, the REIT acknowledges that changes in borrowing costs could impact its financial performance. Effective management of cash flows and operational expenses will be crucial in navigating these economic challenges. Moreover, the company’s commitment to transparency in financial reporting and robust governance practices will continue to enhance stakeholder confidence and support sustainable growth.
+## Strategic Initiatives
+Fortune REIT's strategic initiatives include a focus on community engagement through tenant diversification, enhancing customer experiences with family-oriented activities, and optimizing property management practices to improve operational efficiency. The integration of amenities and services tailored to community needs reflects a commitment to creating attractive retail environments that resonate with local consumers.
+## Risks and Challenges
+Investing in Fortune REIT carries inherent risks, including market volatility, regulatory compliance challenges, and operational risks associated with property management. The ongoing pressures in the retail sector, particularly from e-commerce competition and changing consumer preferences, necessitate a vigilant approach to risk management and market adaptation.
+## Conclusion
+In summary, Fortune REIT’s financial performance in the first half of 2024 underscores both the challenges and opportunities within the retail sector. While experiencing a downturn in revenue, the company’s proactive management and strategic focus on asset enhancement and community engagement position it favorably for future growth. Investors should remain cognizant of the changing market dynamics while recognizing the REIT’s commitment to maintaining transparency, stability, and long-term value creation.
+## Recommendations for Investors
+Potential investors should consider the regulatory compliance, financial stability, and governance practices of Fortune REIT. The emphasis on transparent reporting, strong operational controls, and strategic growth initiatives offers a compelling case for investment. Monitoring the evolving retail landscape and the REIT's responsive strategies will be critical in assessing its future performance and investment viability.</t>
   </si>
   <si>
     <t># Financial Analysis Report
@@ -216,26 +200,58 @@
 As China Longyuan Power Group Corporation continues to navigate a complex market landscape, its commitment to sustainability, operational excellence, and strategic innovation will be instrumental in achieving its ambitious growth objectives. By maintaining agility and responsiveness to market changes, the company can secure its position as a leader in the global energy sector.
 ## 20. Appendices
 Further details, including financial statements, performance metrics, and strategic initiatives, can be provided upon request for a comprehensive understanding of the company's operational performance and future outlook.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>### Financial Analysis Report: Fortune REIT
+  </si>
+  <si>
+    <t># Financial Analysis Report
+## Company Overview
+China Longyuan Power Group Corporation Limited is a leading player in the renewable energy sector, especially focusing on wind and photovoltaic power. The company is strategically positioned to leverage China's transition towards sustainable energy sources. In the first half of 2024, China’s economy experienced a stable growth trajectory, with GDP increasing by 5.0% year-on-year. This economic backdrop supports the company's initiatives, primarily aimed at expanding renewable energy capacity and enhancing operational efficiencies. The company’s strategic emphasis on innovation, talent development, and environmental sustainability aligns with global trends towards green energy adoption.
+## Revenue Structure
+The revenue structure of China Longyuan Power for the first half of 2024 included various segments, such as energy storage equipment rental, repair services, sales of commodity materials, and miscellaneous income. While specific revenue figures were not disclosed for each component, the overall operating profit from these activities reached RMB 101 million—a notable increase of RMB 93 million compared to the same period in 2023. This growth was primarily driven by the company's diversified revenue streams, underlining its commitment to optimizing its financing structure to support revenue-generating activities. However, the report also highlighted challenges in domestic demand that could potentially stifle future revenue growth.
+## Profit
+The company’s net profit performance can be assessed against the backdrop of China's stable economic growth. Despite the favorable conditions, the company faces challenges stemming from insufficient domestic demand and the need for a consolidated economic recovery. These factors could impact net profit sustainability over time. The strategic focus on building a world-class new energy asset management platform aims to capitalize on emerging market opportunities, even as external complexities present potential risks to profitability in the near term.
+## Valuation
+As of June 30, 2024, the company's total liabilities amounted to RMB 80,011 million, with total equity attributable to equity holders at RMB 72,658 million, yielding a debt-to-equity ratio of approximately 1.10. This ratio indicates that the company operates with a relatively leveraged financial position. The valuation metrics suggest that while the company is growing, its reliance on debt financing could pose risks, particularly in a fluctuating economic environment. 
+## Summary
+In summary, China Longyuan Power is navigating a complex economic landscape characterized by growth in renewable energy demand and significant challenges in achieving domestic sales targets. While the revenue structure shows promise through diverse streams, the company's reliance on coal and thermal power raises concerns about sustainability. The focus on enhancing operational efficiency and expanding renewable capacity is crucial for maintaining competitive advantage.
+## Future Outlook
+Looking ahead, China Longyuan Power aims to expand its installed capacity, building on the success of adding 2,286.73 MW across 47 new projects in the first half of 2024. The company’s commitment to optimizing management practices for its existing assets and enhancing its renewable energy portfolio aligns with industry trends towards sustainability. However, it must also navigate external factors such as fluctuating fuel prices, regulatory changes, and market competition which could disrupt growth strategies.
+## Factors Affecting Revenue
+Key factors influencing the company's electricity sales revenue include the introduction of a time-of-use electricity fee policy, which introduces price volatility. The targeted utilization rate for new energy sources aims to remain above 90%, though regional disparities in resource conditions may challenge this goal. Moreover, the pricing mechanisms for ancillary services and fluctuations in coal prices significantly affect electricity sales revenue. 
+## Installed Capacity Trends
+As of June 30, 2024, the company’s consolidated installed capacity reached 37,880.40 MW, reflecting growth attributed to new wind and photovoltaic projects. The expansion in renewable energy infrastructure, particularly photovoltaic technology, is a positive trend for the company, positioning it well for future energy production demands. 
+## Electricity Sales Performance
+In the first half of 2024, total electricity sales declined by 2.39% year-on-year, amounting to 4,907,935 MWh. This decline is attributed to increased competition from new energy capacity in regions like Jiangsu, which has affected coal power generation. The average utilization hours for coal power also fell by 64 hours year-on-year, indicating challenges in maintaining revenue from conventional energy sources.
+## Operational Costs and Profit Margins
+The increase in operational costs, primarily driven by higher personnel expenses and maintenance costs, emphasizes the need for improved efficiency. The operating expenses rose to RMB 2,358 million, reflecting an 8.1% increase compared to the previous year. These pressures on operational costs could negatively impact net profit margins unless effectively managed through strategic cost allocation and operational optimization.
+## Risks and Mitigation Strategies
+The company has identified several operational risks, including weaknesses in grid infrastructure and price volatility from time-of-use electricity fees. To mitigate these risks, the company has implemented robust safety management systems and proactive financial risk assessments, especially concerning foreign exchange and fuel price fluctuations. 
+## Capital Expenditures and Financial Stability
+Increased capital expenditures have implications for financial stability, particularly if funded through debt. The company's approach to capital management, including the integration of newly acquired subsidiaries, further demonstrates a focus on maintaining a steady financial position while pursuing growth opportunities.
+## Regulatory Environment
+The regulatory landscape plays a crucial role in shaping the company’s operations and financial planning. Compliance with accounting standards and adherence to policies regarding renewable energy development are fundamental to the company's strategy and financial reporting processes.
+## Stakeholder Communication
+China Longyuan Power effectively communicates its value proposition to stakeholders by emphasizing its commitment to sustainable growth and innovation. This approach not only strengthens stakeholder relationships but also reinforces the company's market position as a leader in the transition to renewable energy.
+## Conclusion
+In conclusion, China Longyuan Power Group Corporation Limited stands at a pivotal point in its growth trajectory, balancing the opportunities presented by China’s commitment to renewable energy with the challenges of market volatility and operational efficiency. Strategic investments, effective risk management, and a focus on sustainable practices will be essential for the company to navigate the evolving energy landscape and achieve its long-term objectives.</t>
+  </si>
+  <si>
+    <t>### Financial Analysis Report
 #### 1. Company Overview
-Fortune REIT is a prominent real estate investment trust (REIT) primarily focused on the management and operation of retail properties. It operates under a structured governance framework designed to ensure accountability, transparency, and effective risk management. Managed by ESR Asset Management (Fortune) Limited, part of the ESR Group, Fortune REIT aligns its strategies with the interests of its investors, notably Cheung Kong Holdings, which holds a significant 33.34% stake in the REIT. The organization emphasizes compliance with the REIT Code, the Securities and Futures Ordinance (SFO), and the Listing Rules, ensuring that mandatory disclosure obligations are met and that shareholder value is maximized within a regulated environment.
+The company under analysis has demonstrated a commitment to growth and innovation within the renewable energy sector, marking a significant focus on sustainable energy solutions. In the first half of 2024, the company launched 47 new projects, signaling its proactive approach to expanding its operational footprint. During this period, the Gross Domestic Product (GDP) of the region increased by 5.0% year-on-year, suggesting a stable economic environment conducive to development. However, the company did not disclose specific revenue figures or growth rates, indicating a cautious financial management approach amidst external complexities.
 #### 2. Revenue Structure
-In the first half of 2024, Fortune REIT reported a gross revenue of HK$871.8 million, reflecting a 4.1% decrease from HK$908.7 million in the same period in 2023. This decline was primarily driven by negative rental reversions in specific sectors, particularly real estate agencies and supermarkets. The net property income also fell by 5.8% year-on-year to HK$633.1 million from HK$671.9 million. The overall cost-to-revenue ratio increased to 25.1% from 23.8%, indicating rising operational costs amidst declining revenues. Such trends underscore the challenges faced in the retail market, which is still recovering from the impacts of economic fluctuations and changing consumer preferences.
+While the company’s revenue structure lacks detailed disclosure, it can be inferred that significant components include electricity sales from various energy sources, particularly wind and photovoltaic (solar) power. The recent introduction of the coal-fired power capacity tariff mechanism and time-of-use electricity fee policy has impacted pricing and revenue stability. Capital commitments primarily related to the construction of new power projects and renovation of existing plants suggest a focus on energy generation as a significant revenue source. Additionally, the ability to issue corporate bonds indicates potential revenue from financing activities.
 #### 3. Profit
-Fortune REIT's profit metrics reveal a concerning trend as the net property income, defined as the income generated from retail properties after deducting property-related expenses, declined to HK$633.1 million. The property operating expenses increased by 1.4% to HK$219.1 million, further straining profitability. The overall retail sales value decreased by 6.6%, exacerbating the impact on rental income and contributing to the increased cost-to-income ratio. These financial indicators reflect the challenges faced by the REIT in maintaining profitability amidst a competitive and evolving retail landscape.
+The company faced challenges in net profit performance, reporting a decline of 19.6% in the first half of 2024—RMB 4,692 million compared to RMB 5,837 million in the same period of 2023. This downturn highlights difficulties in sustaining profitability amidst a complex external environment and insufficient domestic demand. The ongoing fragility of economic recovery demands enhanced effective demand, posing risks to future profit margins. The disposal of the equity interest in Jiangyin Sulong may have implications for future profitability, as the company adjusts its strategic focus.
 #### 4. Valuation
-The current valuation of Fortune REIT’s properties remains stable, with capitalization rates holding steady at 4.3%. However, the total investment property value slightly decreased from HK$38.439 billion to HK$38.167 billion. This marginal decline indicates potential vulnerabilities in the property valuation due to market dynamics. The management’s proactive strategies to enhance property values, such as the HK$300 million investment in +WOO Phase 2, aim to rejuvenate the asset portfolio and potentially drive future appreciation. Nevertheless, external factors like interest rate changes could significantly impact financing costs and overall property valuations.
+The company's current debt-to-equity ratio stands at approximately 1.81, indicating a relatively high level of leverage, with total liabilities amounting to RMB 148,422,231 against total equity of RMB 82,221,994. This ratio suggests that for every RMB 1 of equity, there is about RMB 1.81 in debt, which may raise concerns among investors regarding financial stability. While leveraging can enhance growth opportunities, it also introduces risks, especially in a fluctuating market environment. The company’s valuation will be influenced by its ability to manage these risks while pursuing growth.
 #### 5. Summary
-The financial performance of Fortune REIT in the first half of 2024 illustrates a decline in both revenue and net property income, driven by various market challenges. The necessary emphasis on effective governance, adherence to regulatory frameworks, and strategic asset management remains vital in navigating these circumstances. With a focus on enhancing tenant mix and occupancy rates, the REIT is working to stabilize its financial health despite the observed downturn in profitability.
+In summary, the company has established itself as a significant player in the renewable energy sector, with a strategic focus on expanding its operational capacity through new projects. However, challenges such as declining net profit, high leverage, and uncertainties in revenue generation from electricity sales raise concerns about its financial health. The company's ability to navigate the complexities of the market, coupled with proactive management of operational costs and capital expenditures, will be crucial for sustaining growth and profitability.
 #### 6. Future Outlook
-Looking ahead, Fortune REIT faces a mixed outlook. While the occupancy rate has shown slight improvement to 94.8%, the retail sector in Hong Kong remains under pressure from economic fluctuations and changing consumer behaviors. The REIT's long-term strategy includes diversifying its tenant mix to include more lifestyle and entertainment offerings, which aligns with evolving community needs. Additionally, government initiatives aimed at boosting retail demand may provide further support. However, challenges such as negative rental reversions in certain sectors could continue to influence rental income stability.
-#### 7. Additional Details
-Fortune REIT's approach towards maintaining high property standards involves engaging independent external valuers for regular assessments, ensuring transparency and accuracy in property valuations. The focus on community-related tenants has enhanced the shopping experience and attracted diverse demographics, contributing to an increased occupancy rate. Furthermore, effective management of operational costs, alongside strategic leasing agreements, is crucial for sustaining profitability. Investor relations are strengthened through transparency in financial reporting and regular updates on corporate governance practices, fostering trust and confidence among stakeholders.
-In conclusion, while Fortune REIT is navigating a challenging environment marked by fluctuating revenues and competitive pressures, its proactive governance and strategic initiatives position it for resilience and potential growth in the evolving retail landscape.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+Looking ahead, the company aims to adapt to changing market conditions by optimizing project layouts across 31 provincial-level regions in China. It is also focused on enhancing operational efficiency through digital transformation and innovative safety management practices. The emphasis on developing offshore wind projects and increasing green electricity trading indicates a commitment to expanding its renewable energy contributions. However, external factors such as regulatory changes, geopolitical risks, and market fluctuations could disrupt growth strategies, necessitating effective risk management and contingency plans.
+#### 7. Additional Insights
+The company’s electricity sales volume increased by 14.1% year-on-year in 2023, driven by significant growth in wind and solar power sales. Nevertheless, average utilization hours for wind power decreased by 101 hours in the first half of 2024 due to reduced wind resources, impacting revenue generation in this segment. The operational challenges, including rising repair and maintenance expenses and increased depreciation costs, further complicate the financial landscape.
+Additionally, subsidy receivables play a vital role in the company’s financial health, providing liquidity and enhancing cash flow stability. As of June 30, 2024, the company is optimistic about recovering subsidies related to its projects, which could bolster future revenue streams. However, reliance on subsidies poses risks, making effective management of receivables critical.
+In conclusion, the company’s strategic direction aligns with industry developments towards sustainable energy solutions, but it must address several challenges to enhance its competitive position. The focus on innovation, operational efficiency, and proactive risk management will be essential for navigating the evolving market landscape and achieving long-term growth objectives.</t>
   </si>
   <si>
     <t># Financial Analysis Report: JNBY
@@ -261,7 +277,43 @@
 6. **Global Trade Dynamics**: The implications of global trade dynamics, including changes in economic climate and trade relations, will require JNBY to remain agile in its operational strategies. Monitoring these external factors will be crucial for sustaining its growth and navigating potential disruptions.
 7. **Sustainability Initiatives**: JNBY's dedication to sustainable practices, including the use of eco-friendly materials and charitable contributions, positions it favorably among environmentally conscious consumers. This commitment will be instrumental in building long-term brand loyalty and trust.
 In conclusion, JNBY's strong financial performance, coupled with its strategic focus on sustainability and innovation, presents a promising outlook for the company as it continues to adapt to the evolving retail landscape. Stakeholders should remain engaged in monitoring JNBY's initiatives and market developments as the company strives to achieve its long-term objectives.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t># JNBY Financial Analysis Report
+## Company Overview
+JNBY, an influential designer fashion house based in China, has been operational for nearly three decades, establishing itself as a prominent player in the contemporary apparel market. The company's diverse brand portfolio includes established names like JNBY, along with younger and emerging brands such as CROQUIS, jnby by JNBY, and POMME DE TERRE. This segmentation allows JNBY to effectively target distinct customer demographics with tailored products, ranging from apparel to footwear and household items. As of June 30, 2024, JNBY has adapted to the evolving landscape of digital consumption and e-commerce, reflecting a commitment to quality and customer experience. This adaptation is critical, given the growing trend of consumers gravitating towards trusted brands that offer personalized experiences.
+## Revenue Structure
+JNBY's revenue structure is significantly influenced by its diversified brand portfolio and sales channels. The company primarily generates revenue from offline retail outlets and online platforms, with Tmall.com being a notable third-party platform for e-commerce. For the fiscal year ending June 30, 2024, JNBY reported total revenue of RMB 5,238,149, marking a 17.3% increase from RMB 4,465,124 in the previous year. This growth can be attributed to both the expansion of standalone retail stores from 1,990 to 2,024 and a notable increase in same-store sales. The integration of a loyalty program has further enhanced revenue generation by encouraging repeat purchases, indicating that JNBY is effectively leveraging both its physical and digital sales channels.
+## Profit
+In terms of profitability, JNBY has demonstrated strong performance metrics. The company's gross profit for the same fiscal year increased to RMB 3,470,485 from RMB 2,916,992, reflecting a growth rate of approximately 19%. This outpaced revenue growth, suggesting improved operational efficiency and effective cost management strategies. Notably, JNBY's operating profit surged to RMB 1,194,266, a remarkable increase of 39.5% from RMB 857,898 in the prior year. This indicates a favorable trend in profitability, as the net profit growth significantly outpaced gross profit growth, showcasing the company's ability to capitalize on increased sales while managing expenses effectively.
+## Valuation
+The valuation of JNBY can be inferred through its financial performance indicators and market positioning. The increasing trend in dividends, with a total payout of HK$1.71 per ordinary share for the 2024 fiscal year, signals confidence in sustained growth and profitability. This includes a final dividend of HK$0.86, an interim dividend of HK$0.46, and a special interim dividend of HK$0.39, representing a clear commitment to returning value to shareholders. The overall increase in dividends compared to the previous fiscal year aligns with JNBY's focus on high-quality development and reflects the company's positive outlook on consumption growth.
+## Summary
+Overall, JNBY's financial performance for the fiscal year ending June 30, 2024, demonstrates resilience and adaptability in a competitive market. The company's revenue growth, coupled with substantial increases in both gross and operating profits, highlights effective management strategies and a commitment to operational excellence. JNBY's diversified brand portfolio and multi-channel sales approach position it favorably in the evolving fashion landscape, where consumer preferences are shifting towards sustainability and personalized experiences. 
+## Future Outlook
+Looking ahead, JNBY's management anticipates continued revenue growth, driven by the stabilization of China's economy and a renewed focus on expanding domestic demand. Enhanced consumer confidence is expected to bolster sales, particularly as the company adapts to changing consumer behaviors through its "design-driven" approach and multi-brand strategies. Additionally, JNBY's emphasis on sustainability and social responsibility is likely to resonate with younger consumers, further enhancing its market position.
+Strategically, JNBY plans to recruit talent with expertise in brand management to support its expansion into new product categories, including children's apparel and household goods. This diversification, alongside their commitment to quality and innovative design, positions JNBY for sustainable growth in the coming years.
+## Other Details
+JNBY's commitment to sustainability is evident through its focus on eco-friendly materials and supplier management practices that prioritize green energy. The company has engaged actively in industry discussions on sustainable development, indicating its alignment with global trends toward responsible consumption. Financially, JNBY's proactive risk management strategies, including its approach to market and operational risks, contribute to its resilience against external shocks.
+In conclusion, JNBY is well-positioned for future growth, supported by a robust financial framework, a commitment to sustainability, and an adaptive approach to market changes. The company's focus on innovation, customer engagement, and operational efficiency will be key to navigating the competitive landscape and achieving long-term success.</t>
+  </si>
+  <si>
+    <t># Financial Analysis Report for JNBY
+## 1. Company Overview
+JNBY, a leading designer brand fashion house established in China, specializes in contemporary apparel, footwear, accessories, and household products. As of June 30, 2024, JNBY's portfolio includes a range of brands from its mature flagship brand (JNBY) to younger brands like CROQUIS, jnby by JNBY, and LESS, alongside emerging brands such as POMME DE TERRE and onmygame. The company's strategic approach focuses on catering to distinct customer segments through diverse design identities, with the recent launch of a children's apparel line, onmygame, further broadening its consumer base. By targeting various age groups and emphasizing diverse design philosophies, JNBY positions itself as a versatile entity in the competitive fashion landscape.
+## 2. Revenue Structure
+JNBY's revenue structure is primarily derived from its diversified brand portfolio. For the fiscal year 2024, the company reported total revenues of RMB 5,238 million, reflecting a robust growth rate of 17.3%. This increase is attributed to the stabilization of China's economy, renewed consumer confidence, and the company's commitment to sustainable development. The integration of both offline and online sales channels has also contributed to revenue generation, with the rise of e-commerce platforms like Tmall.com complementing traditional retail operations. JNBY's sales channels are strategically diversified, enabling the company to optimize consumer reach and enhance overall sales performance.
+## 3. Profit
+JNBY's profit performance for Fiscal Year 2024 showed significant growth, with net profit reaching RMB 848 million, an impressive increase of 36.5%. However, this growth came alongside a gross profit of RMB 3,470.5 million, which saw a rise of approximately 49.4%. Despite the positive trends in revenue and net profit, challenges remain in maintaining profit margins due to competitive pressures and fluctuating consumer confidence. The observed discrepancies between gross and net profit growth suggest that while the top-line performance is strong, operational costs and financial expenses may be constraining overall profitability.
+## 4. Valuation
+The company's valuation reflects its commitment to sustainable growth and shareholder returns. JNBY’s focus on enhancing operational and financial systems contributes to its long-term investment appeal. The increased demand for locally sourced fashion brands in China further enhances JNBY's valuation, particularly as the company aligns its operational strategies with market preferences. As of the latest reporting, the company has made strides in maintaining its competitive edge, which is essential for sustaining its market valuation amid changing economic conditions.
+## 5. Summary
+In summary, JNBY has demonstrated resilience in its financial performance, with notable revenue and profit growth amid a recovering economic environment. The company's diversified brand portfolio and strategic multi-channel sales approach have positioned it favorably within the fashion industry. While revenue growth is commendable, the challenges of maintaining profit margins and managing operational costs will require ongoing attention. JNBY's commitment to sustainability and social responsibility further enhances its brand image, making it a compelling player in the competitive landscape.
+## 6. Future Outlook
+Looking ahead, JNBY is well-positioned for continued growth. The company's strategic priorities include enhancing product offerings, particularly in personalized and sustainable products, to meet the evolving preferences of younger consumers. As digital consumption rises, JNBY is likely to continue advancing its e-commerce initiatives and integrating online and offline retail experiences. Management's expectations for revenue growth are optimistic, supported by potential increases in gross merchandise value (GMV) and a commitment to innovation. However, external market factors, including economic fluctuations and competitive pressures, will require careful navigation.
+## 7. Other Details
+JNBY's operational strategies also encompass detailed risk management approaches, particularly concerning financial liabilities and market risks. The company's emphasis on supplier relationships, employee training, and operational resilience underscores its commitment to sustained performance. Furthermore, JNBY actively engages in corporate social responsibility initiatives, contributing to community welfare and environmental sustainability. By fostering a culture of transparency and accountability, JNBY aims to build robust stakeholder relations and enhance its corporate governance practices.
+In conclusion, JNBY's holistic approach to managing its business operations, combined with a focus on sustainable growth and innovation, positions it favorably for the future. Continuous monitoring of market dynamics, consumer behavior, and operational efficiency will be crucial for JNBY to maintain its competitive advantage and achieve long-term success in the fashion industry.</t>
   </si>
   <si>
     <t># Financial Analysis Report of China Tobacco International
@@ -290,7 +342,73 @@
 Technological innovation plays a significant role in CTI's operations. The company has invested in upgrading its ERP system to optimize operational efficiency and reduce costs. Furthermore, the focus on product innovation and enhancing customer engagement through digital channels is indicative of the company's commitment to leveraging technology for competitive advantage.
 ### Conclusion
 In conclusion, China Tobacco International stands at a pivotal juncture within the tobacco industry, characterized by evolving market dynamics and changing consumer preferences. While the company has successfully increased revenue, the challenges posed by shifting product margins necessitate a strategic focus on enhancing profitability. By leveraging its competitive advantages, managing risks effectively, and embracing innovation, CTI is well-positioned to navigate the complexities of the tobacco market and achieve sustainable growth in the years to come.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t># Financial Analysis Report: China Tobacco International (HK) Company Limited
+## 1. Company Overview
+China Tobacco International (HK) Company Limited (CTIHK) functions as a pivotal subsidiary of the China National Tobacco Corporation (CNTC). It specializes in the import and export of tobacco leaf products, thereby playing a critical role in international trade within the tobacco industry. In 2024, CTIHK engaged in substantial transactions, recording HK$1,461.3 million under its tobacco purchase agreements. This figure highlights the company's robust operational capacity and strategic significance within CNTC's broader framework. The company's ownership structure indicates a significant relationship with its parent entity, China Tobacco International Group (CTIG), which suggests that CTIG likely exerts considerable control over CTIHK's operations.
+## 2. Revenue Structure
+CTIHK’s revenue is primarily derived from its Tobacco Leaf Products Export and Import businesses. In the first half of 2024, the Tobacco Leaf Products Import Business reported total revenue of HK$6,802.2 million, representing the entirety of its revenue stream. This indicates a well-structured business model that focuses on long-term supply agreements with strategic partners such as Alliance One Brazil. The export segment further diversifies revenue, targeting key markets including Southeast Asia, Hong Kong, Macau, Taiwan, and Europe. The sales dynamics demonstrate the company's ability to adapt its offerings to meet market demands effectively.
+## 3. Profit
+The company achieved a remarkable 33% increase in profit for the period, amounting to HK$679,702 million, up from HK$510,540 million in the previous year. Despite this growth in profit, there was a noted decline in gross profit margins due to a shift in product sales towards finished tobacco strips, which, although higher in unit price, offered lower gross margins compared to traditional tobacco leaf by-products. The total sale transactions during the reporting period reached HK$184.0 million, further underscoring CTIHK's operational performance amidst changing market dynamics.
+## 4. Valuation
+While specific valuation metrics for CTIHK relative to industry standards are not detailed within the retrieved context, the company’s profitability, along with its substantial revenue figures, suggests a potentially favorable valuation position. Typically, valuation assessments involve analyzing price-to-earnings (P/E) ratios, price-to-sales (P/S) ratios, and enterprise value-to-EBITDA (EV/EBITDA) ratios. The increase in profit and revenue, coupled with strategic growth plans, positions CTIHK favorably within the market, likely leading to a positive outlook on its valuation in the tobacco sector.
+## 5. Summary
+In summary, CTIHK has positioned itself as a significant player in the international tobacco market through its comprehensive procurement, export, and import operations. The company's financial performance has been robust, highlighted by a notable increase in profit alongside strategic revenue generation from both its export and import businesses. However, challenges remain, particularly concerning gross profit margins, which require close monitoring and strategic adjustments to ensure sustained profitability.
+## 6. Future Outlook
+Looking ahead, CTIHK anticipates continued growth driven by its strategic focus on both organic and inorganic development. The company's commitment to enhancing its market presence through innovative product offerings, particularly in the new tobacco products segment, signals a proactive approach to capturing market share. The increase in revenue from new tobacco products, from HK$33,895,000 in 2023 to HK$43,517,000 in 2024, reflects the company's adaptability to consumer trends. Furthermore, the absence of export tariffs for new tobacco products is expected to bolster competitiveness in international markets.
+## 7. Operational and Strategic Insights
+CTIHK's operational strategy is underpinned by a diversified supply chain management approach, allowing for effective resource allocation across its various business segments. The company engages in rigorous market analysis to adapt its pricing strategies based on supply chain dynamics, customer demand, and market conditions. This flexible approach is critical in managing fluctuations in procurement costs and maintaining profitability.
+Moreover, CTIHK's emphasis on corporate governance enhances its operational transparency and compliance with regulatory standards. The company’s adherence to the Hong Kong Financial Reporting Standards (HKFRS) and the Companies Ordinance demonstrates a commitment to maintaining high standards of corporate governance, which is vital for fostering stakeholder trust.
+## 8. Performance Monitoring and Risk Management
+CTIHK employs a structured performance monitoring system through segment reporting that evaluates the revenue from different product lines and geographical regions. This allows for a granular assessment of profitability and operational efficiency. The company is also aware of potential risks, including fluctuations in global tobacco supply, regulatory changes, and shifting consumer preferences towards alternative products. To mitigate these risks, CTIHK engages in long-term partnerships with approved suppliers, ensuring a stable supply chain and consistent product quality.
+## 9. Conclusion
+In conclusion, China Tobacco International (HK) Company Limited is strategically positioned within the global tobacco industry, demonstrating robust financial performance amid evolving market conditions. The company’s focus on sustainable growth through innovative product development and strategic partnerships enables it to navigate challenges while capitalizing on emerging opportunities. As it continues to adapt to changing consumer demands and market dynamics, CTIHK is well-positioned for sustained success in the years to come.</t>
+  </si>
+  <si>
+    <t># Financial Analysis Report of China Tobacco International
+## 1. Company Overview
+China Tobacco International (CTI) operates as a subsidiary of the China National Tobacco Corporation (CNTC), the world's largest tobacco company. Primarily engaged in the export and import of tobacco leaf products, CTI plays a vital role in facilitating the global distribution of tobacco to key markets, particularly in Southeast Asia and Europe. The company’s operational framework includes strategic partnerships, such as the Framework Tobacco Sales Agreement with Alliance One International, which enhances its supply chain capabilities and market reach. Despite its significant role within the CNTC framework, explicit details regarding its ownership structure remain scarce, indicating a potential state-owned model typical of the Chinese tobacco industry.
+## 2. Revenue Structure
+CTI's revenue generation is diversified across several key segments: Tobacco Leaf Products Export Business, Tobacco Leaf Products Import Business, Cigarettes Export Business, New Tobacco Products Export Business, and operations in Brazil. The company strategically positions itself by focusing on high-quality tobacco leaf procurement and establishing strong relationships with suppliers and merchants. In 2024, the company reported an increase in revenue attributable to higher sales volumes of finished tobacco strips, which, despite lower gross profit margins, reflect a proactive adjustment in response to market demand.
+## 3. Profit
+The profitability landscape of CTI is shaped by its product mix and operational strategies. The company has noted a shift towards finished tobacco strips, which, while yielding higher unit prices, have lower gross profit margins compared to tobacco leaf by-products. For the first half of 2024, the gross profit margin was adversely affected by this product mix shift, leading to an overall decrease in gross profit despite increased revenue. The current profit attributable to equity shareholders rose by 41%, highlighting the company’s effective cost management and revenue optimization strategies amid changing market conditions.
+## 4. Valuation
+CTI's valuation is influenced by its operational performance and market dynamics. The absence of domestic reference pricing for certain tobacco products complicates direct comparisons with industry standards. Instead, the company relies on arm's length negotiations with suppliers and customers to determine pricing, which incorporates various operational costs. This flexible pricing strategy allows CTI to adapt to market fluctuations while ensuring competitive positioning. However, the lower net margins, particularly in the New Tobacco Products Export Business, necessitate ongoing monitoring to uphold financial stability.
+## 5. Summary
+CTI operates within a complex industry landscape characterized by stringent regulations and intense competition. Its revenue structure reflects a proactive approach to market demands, though challenges persist regarding gross profit margins due to product mix changes. The company's strategic partnerships and operational efficiencies contribute positively to its financial performance, even as it navigates the intricacies of the international tobacco market. A cautious yet optimistic outlook suggests that CTI is well-positioned to sustain its growth trajectory.
+## 6. Future Outlook
+Looking ahead, CTI aims to bolster its market share by enhancing strategic relationships and exploring new opportunities in the evolving tobacco landscape. With a focus on high-quality development and international expansion, the company is well aware of the potential for growth in the new tobacco products segment. Strategic agreements, such as those with Alliance One International, will likely play a pivotal role in enhancing distribution channels and accessing new markets. However, the company must remain vigilant regarding pricing strategies and market conditions to ensure sustained profitability.
+## 7. Other Details
+### Supply Chain Management
+CTI effectively manages its supply chain for exports through strategic procurement of various grades of tobacco leaves, ensuring a steady supply to meet diverse customer demands. The company’s collaborations with suppliers like Alliance One Brazil enhance its procurement capabilities and mitigate risks associated with extreme weather and shipping fluctuations. 
+### Pricing Strategy
+The pricing strategy for tobacco leaf imports is influenced by supplier costs, market conditions, and competitive pricing dynamics. CTI aims to maintain a minimum margin of 1% in its New Tobacco Products Export Business, reflecting a careful assessment of operational costs and market demand.
+### Risk Management
+CTI faces several potential risks, including fluctuations in international market conditions, reliance on specific regional markets, and competition from established brands. To mitigate these risks, the company employs a structured approach to pricing, ensuring flexibility amidst changing market dynamics. Additionally, ongoing compliance with regulatory standards remains a critical focus.
+### Corporate Governance and ESG
+Strong corporate governance practices are integral to CTI's operational strategy, ensuring transparency and ethical decision-making. The company's commitment to sustainability is reflected in its ongoing efforts to enhance its ESG performance, which may improve brand reputation and investor confidence.
+### Conclusion
+In summary, China Tobacco International stands as a formidable player in the tobacco industry, with diverse revenue streams and strategic initiatives aimed at sustaining its market presence. While challenges related to product mix and market conditions persist, the company's proactive approach to governance, sustainability, and operational efficiency positions it favorably for future growth. As it navigates the complexities of the global tobacco market, CTI's focus on innovation and strategic partnerships will be crucial in maintaining its competitive edge and driving long-term profitability.</t>
+  </si>
+  <si>
+    <t># Financial Analysis Report of CK Hutchison Holdings Limited
+## Company Overview
+CK Hutchison Holdings Limited operates as a diversified multinational conglomerate with a primary business structure organized into four core segments: ports and related services, retail, infrastructure, and telecommunications. This segmentation allows senior executive management to monitor performance and allocate resources effectively, which enhances strategic decision-making within each core area. By leveraging its extensive management experience across sectors and geographies, the company pursues organic growth while actively engaging in merger and acquisition activities to further diversify its operations.
+## Revenue Structure
+The company’s revenue structure is categorized into traditional service offerings while also expanding into new revenue streams. The telecommunications segment, for instance, has seen growth through active customer base expansion and new offerings, including cybersecurity and insurance products. In contrast, its retail segment faces challenges due to a mix of low-margin Internet of Things (IoT) customers and inflation-linked customer contract adjustments. Revenue performance varies significantly across geographical regions, with Sweden experiencing a 6% increase in total margin driven by customer growth, while Hutchison Telecommunications Hong Kong encountered a 12% decline in total revenue due to shifting consumer spending patterns.
+## Profit
+Profitability across CK Hutchison's segments has shown mixed results. The company reported a 5% increase in EBITDA, reflecting operational improvements in its Ports and telecommunications divisions. However, the infrastructure segment has faced challenges, notably due to a tariff reset and rising energy costs in the UK and Europe, which have negatively impacted revenue and profit margins. The retail segment's performance is also under scrutiny, particularly in Health and Beauty China, where comparable store sales declined by 19%. Overall, while some segments thrive, others struggle, highlighting the necessity for disciplined management of costs and margins to enhance long-term returns for stakeholders.
+## Valuation
+Valuation metrics indicate that CK Hutchison Holdings Limited maintains a solid financial profile, with a total capital ratio improving to 17.1% from 16.2%. This improvement suggests stronger financial health and stability. The company's focus on achieving recurring and sustainable earnings supports its valuation, alongside its commitment to maintaining long-term investment-grade ratings. However, challenges remain in certain segments, which could influence market perceptions and future valuations. The group’s strategic investments in technology and infrastructure aim to bolster its overall market position, ensuring that valuation remains aligned with long-term growth prospects.
+## Summary
+In summary, CK Hutchison Holdings Limited exhibits a diverse business model with segmented operations that allow for targeted management and strategic growth. While the company has achieved substantial growth in certain areas, it faces challenges in others, particularly in its retail and infrastructure segments. The mixed performance underscores the necessity for ongoing evaluation of market conditions and operational efficiencies, alongside proactive measures to enhance profitability across divisions.
+## Future Outlook
+Looking ahead, CK Hutchison Holdings Limited is poised to navigate a complex market landscape characterized by economic uncertainties and competitive pressures. The demand outlook remains positive for the third quarter, although a gradual slowdown is anticipated due to frontloaded cargo orders for the holiday season. The company plans to leverage its strengths in technology transformation and operational enhancements to capture new revenue opportunities, particularly in sectors where it has established management expertise and resources. Additionally, the emphasis on sustainability through initiatives like decarbonization and the "Equipment Electrification Directive" reflects the company’s commitment to align its operations with evolving market demands.
+## Other Details
+Key performance indicators are essential for CK Hutchison's ongoing evaluation of its business segments, with a focus on recurring earnings, cash flow, and dividend growth. Management’s disciplined approach to revenue growth, margin management, and cost control will be pivotal in addressing ongoing market challenges. Furthermore, the company's proactive stance on regulatory compliance and risk management enhances its resilience and adaptability in an ever-evolving global marketplace.
+In conclusion, CK Hutchison Holdings Limited's strategic priorities for growth, combined with its commitment to operational efficiency and sustainability, position the company favorably for future success. As it continues to adapt to changing market dynamics, the company must remain vigilant in managing its weaknesses, particularly in the infrastructure and retail segments, to ensure sustained profitability and shareholder value.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -306,16 +424,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="新細明體"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="新細明體"/>
     </font>
   </fonts>
   <fills count="2">
@@ -353,20 +471,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -670,176 +784,187 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="114.125" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="1"/>
+    <col min="1" max="3" width="79.375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="409.6">
+    <row r="2" spans="1:3" ht="409.6">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="109.625" style="3" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="409.6">
-      <c r="A2" s="3" t="s">
+      <c r="C2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="113.75" style="5" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" ht="409.6">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="111.5" style="5" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" ht="409.6">
-      <c r="A2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>2</v>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="114.75" style="5" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" ht="409.6">
-      <c r="A2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>3</v>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>